<commit_message>
1. Handled Same category in Axis category 1 and axis category 2 is not allowing drill down 2. Handled Date formatting 3. Handled cross filtering issue
</commit_message>
<xml_diff>
--- a/documents/Published/Box and Whisker/BoxAndWhiskerByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/Box and Whisker/BoxAndWhiskerByMAQSoftwareChecklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PowerBI-CustomVisuals\documents\Published\BoxAndWhisker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAQUser\source\repos\NewRepo2\documents\Published\BoxAndWhisker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DD3440-92B3-450F-A4CB-3BE44BA08B82}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E743DF-C046-4BD3-98BD-0EE8DA0386B5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945" xr2:uid="{4AB92824-63E9-41E2-A760-A81835BDCF59}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="322">
   <si>
     <t>S no</t>
   </si>
@@ -1228,6 +1228,42 @@
 2. Visual will update according to selections
 3. In the boomarks pane, a new entry of the bookmark will come
 4. The selection state saved in bookmark will be restored in the visual</t>
+  </si>
+  <si>
+    <t>1. Apply some format to date column from modelling tab
+2. Go to category filed in visual 
+3. Drag that column in category field</t>
+  </si>
+  <si>
+    <t>Date Formatting</t>
+  </si>
+  <si>
+    <t>Check whether date formatting works</t>
+  </si>
+  <si>
+    <t>1.Date format is visilble in visual
+2.Format is change from modelling tab visual is updated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drill down </t>
+  </si>
+  <si>
+    <t>Check whether drill down works when same Date field is dragged in Axis Category 1 and Axis Category 2</t>
+  </si>
+  <si>
+    <t>2. Drag Date in Axis Category 2</t>
+  </si>
+  <si>
+    <t>3. Drill Down on Axis Category 1</t>
+  </si>
+  <si>
+    <t>1. Drag Date in Axis Category 1 (Date Hierarchy)</t>
+  </si>
+  <si>
+    <t>1. Drill down works on Axis Category 1</t>
+  </si>
+  <si>
+    <t>2. Drill up works on Axis Category 1</t>
   </si>
 </sst>
 </file>
@@ -1351,7 +1387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1396,6 +1432,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1414,11 +1459,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1737,10 +1784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD979CE-A2F4-4A57-BF74-C680FEBF31B0}">
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" topLeftCell="B82" workbookViewId="0">
+      <selection activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2960,23 +3007,100 @@
       </c>
     </row>
     <row r="87" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A87" s="23">
+      <c r="A87" s="17">
         <v>22</v>
       </c>
-      <c r="B87" s="22" t="s">
+      <c r="B87" s="16" t="s">
         <v>307</v>
       </c>
-      <c r="C87" s="22" t="s">
+      <c r="C87" s="16" t="s">
         <v>308</v>
       </c>
-      <c r="D87" s="24" t="s">
+      <c r="D87" s="18" t="s">
         <v>309</v>
       </c>
-      <c r="E87" s="24" t="s">
+      <c r="E87" s="18" t="s">
         <v>310</v>
       </c>
     </row>
+    <row r="88" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="28">
+        <v>23</v>
+      </c>
+      <c r="B88" s="27" t="s">
+        <v>312</v>
+      </c>
+      <c r="C88" s="25" t="s">
+        <v>313</v>
+      </c>
+      <c r="D88" s="29" t="s">
+        <v>311</v>
+      </c>
+      <c r="E88" s="29" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="28"/>
+      <c r="B89" s="27"/>
+      <c r="C89" s="25"/>
+      <c r="D89" s="29"/>
+      <c r="E89" s="29"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="28"/>
+      <c r="B90" s="27"/>
+      <c r="C90" s="25"/>
+      <c r="D90" s="29"/>
+      <c r="E90" s="29"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="28">
+        <v>24</v>
+      </c>
+      <c r="B91" s="27" t="s">
+        <v>315</v>
+      </c>
+      <c r="C91" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="D91" s="13" t="s">
+        <v>319</v>
+      </c>
+      <c r="E91" s="13" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="28"/>
+      <c r="B92" s="27"/>
+      <c r="C92" s="25"/>
+      <c r="D92" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="E92" s="13" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="28"/>
+      <c r="B93" s="27"/>
+      <c r="C93" s="25"/>
+      <c r="D93" s="13" t="s">
+        <v>318</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="E88:E90"/>
+    <mergeCell ref="C91:C93"/>
+    <mergeCell ref="B91:B93"/>
+    <mergeCell ref="A91:A93"/>
+    <mergeCell ref="D88:D90"/>
+    <mergeCell ref="C88:C90"/>
+    <mergeCell ref="B88:B90"/>
+    <mergeCell ref="A88:A90"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -3172,29 +3296,29 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="16">
+      <c r="A17" s="19">
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="22" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="C18" s="20"/>
+      <c r="C18" s="23"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="18"/>
+      <c r="A19" s="21"/>
       <c r="B19" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="C19" s="21"/>
+      <c r="C19" s="24"/>
     </row>
     <row r="20" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
@@ -3208,41 +3332,41 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="16">
+      <c r="A21" s="19">
         <v>18</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="22" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="C22" s="20"/>
+      <c r="C22" s="23"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
+      <c r="A23" s="20"/>
       <c r="B23" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="C23" s="20"/>
+      <c r="C23" s="23"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
+      <c r="A24" s="20"/>
       <c r="B24" s="9"/>
-      <c r="C24" s="20"/>
+      <c r="C24" s="23"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="18"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="C25" s="21"/>
+      <c r="C25" s="24"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">

</xml_diff>

<commit_message>
Added report tooltip and displayed dots above box.
</commit_message>
<xml_diff>
--- a/documents/Published/Box and Whisker/BoxAndWhiskerByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/Box and Whisker/BoxAndWhiskerByMAQSoftwareChecklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAQUser\source\repos\NewRepo2\documents\Published\BoxAndWhisker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualWork\documents\Published\BoxAndWhisker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E743DF-C046-4BD3-98BD-0EE8DA0386B5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D31E0D-7D70-4AA6-A28C-D96B857BA74F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945" xr2:uid="{4AB92824-63E9-41E2-A760-A81835BDCF59}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945" activeTab="1" xr2:uid="{4AB92824-63E9-41E2-A760-A81835BDCF59}"/>
   </bookViews>
   <sheets>
     <sheet name="BVTs" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="323">
   <si>
     <t>S no</t>
   </si>
@@ -1264,6 +1264,9 @@
   </si>
   <si>
     <t>2. Drill up works on Axis Category 1</t>
+  </si>
+  <si>
+    <t>Is report tooltip working properly?</t>
   </si>
 </sst>
 </file>
@@ -1387,7 +1390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1441,6 +1444,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1458,17 +1478,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1786,7 +1795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD979CE-A2F4-4A57-BF74-C680FEBF31B0}">
   <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B82" workbookViewId="0">
+    <sheetView topLeftCell="B82" workbookViewId="0">
       <selection activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
@@ -3024,44 +3033,44 @@
       </c>
     </row>
     <row r="88" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="28">
+      <c r="A88" s="25">
         <v>23</v>
       </c>
-      <c r="B88" s="27" t="s">
+      <c r="B88" s="24" t="s">
         <v>312</v>
       </c>
-      <c r="C88" s="25" t="s">
+      <c r="C88" s="23" t="s">
         <v>313</v>
       </c>
-      <c r="D88" s="29" t="s">
+      <c r="D88" s="21" t="s">
         <v>311</v>
       </c>
-      <c r="E88" s="29" t="s">
+      <c r="E88" s="21" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="28"/>
-      <c r="B89" s="27"/>
-      <c r="C89" s="25"/>
-      <c r="D89" s="29"/>
-      <c r="E89" s="29"/>
+      <c r="A89" s="25"/>
+      <c r="B89" s="24"/>
+      <c r="C89" s="23"/>
+      <c r="D89" s="21"/>
+      <c r="E89" s="21"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="28"/>
-      <c r="B90" s="27"/>
-      <c r="C90" s="25"/>
-      <c r="D90" s="29"/>
-      <c r="E90" s="29"/>
+      <c r="A90" s="25"/>
+      <c r="B90" s="24"/>
+      <c r="C90" s="23"/>
+      <c r="D90" s="21"/>
+      <c r="E90" s="21"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="28">
+      <c r="A91" s="25">
         <v>24</v>
       </c>
-      <c r="B91" s="27" t="s">
+      <c r="B91" s="24" t="s">
         <v>315</v>
       </c>
-      <c r="C91" s="26" t="s">
+      <c r="C91" s="22" t="s">
         <v>316</v>
       </c>
       <c r="D91" s="13" t="s">
@@ -3072,9 +3081,9 @@
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="28"/>
-      <c r="B92" s="27"/>
-      <c r="C92" s="25"/>
+      <c r="A92" s="25"/>
+      <c r="B92" s="24"/>
+      <c r="C92" s="23"/>
       <c r="D92" s="13" t="s">
         <v>317</v>
       </c>
@@ -3083,9 +3092,9 @@
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="28"/>
-      <c r="B93" s="27"/>
-      <c r="C93" s="25"/>
+      <c r="A93" s="25"/>
+      <c r="B93" s="24"/>
+      <c r="C93" s="23"/>
       <c r="D93" s="13" t="s">
         <v>318</v>
       </c>
@@ -3108,10 +3117,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ED1C0CB-CCB9-4DDC-B99C-E719FAB4C761}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3296,29 +3305,29 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="19">
+      <c r="A17" s="26">
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="29" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="C18" s="23"/>
+      <c r="C18" s="30"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="21"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="C19" s="24"/>
+      <c r="C19" s="31"/>
     </row>
     <row r="20" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
@@ -3332,41 +3341,41 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="19">
+      <c r="A21" s="26">
         <v>18</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="29" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="C22" s="23"/>
+      <c r="C22" s="30"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
+      <c r="A23" s="27"/>
       <c r="B23" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="C23" s="23"/>
+      <c r="C23" s="30"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
+      <c r="A24" s="27"/>
       <c r="B24" s="9"/>
-      <c r="C24" s="23"/>
+      <c r="C24" s="30"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="21"/>
+      <c r="A25" s="28"/>
       <c r="B25" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="C25" s="24"/>
+      <c r="C25" s="31"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
@@ -3387,6 +3396,17 @@
         <v>156</v>
       </c>
       <c r="C27" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="19">
+        <v>21</v>
+      </c>
+      <c r="B28" t="s">
+        <v>322</v>
+      </c>
+      <c r="C28" s="20" t="s">
         <v>132</v>
       </c>
     </row>
@@ -3398,5 +3418,6 @@
     <mergeCell ref="C21:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>